<commit_message>
Añadidos los avisos de la Aemet
</commit_message>
<xml_diff>
--- a/complementarios_lluvias/df_maestro.xlsx
+++ b/complementarios_lluvias/df_maestro.xlsx
@@ -549,17 +549,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>18,3</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -607,17 +607,17 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>35,1</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -711,17 +711,17 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>11,2</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -769,17 +769,17 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,1</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -885,17 +885,17 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Ip</t>
+          <t>4,2</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -943,7 +943,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1117,17 +1117,17 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>2,8</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1175,17 +1175,17 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>0,2</t>
+          <t>0,4</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1233,17 +1233,13 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Ip</t>
-        </is>
-      </c>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1291,17 +1287,17 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Ip</t>
+          <t>0,2</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1349,17 +1345,17 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>1,2</t>
+          <t>2,2</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1403,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1417,7 +1413,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1465,17 +1461,17 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>38,8</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1661,17 +1657,17 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>2,9</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1811,17 +1807,17 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>Ip</t>
+          <t>9,9</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1867,17 +1863,17 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Ip</t>
+          <t>10,1</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1925,17 +1921,17 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>0,8</t>
+          <t>20,4</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -1983,17 +1979,17 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>9,1</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2041,17 +2037,17 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>5,8</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2145,17 +2141,13 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>0,0</t>
-        </is>
-      </c>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
       <c r="N31" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2203,17 +2195,17 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,2</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2261,17 +2253,17 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>0,1</t>
+          <t>1,2</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2363,17 +2355,17 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>0,2</t>
+          <t>1,0</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2421,17 +2413,17 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>6,8</t>
+          <t>0,3</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2479,17 +2471,17 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>5,8</t>
+          <t>0,4</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2537,17 +2529,17 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>1,5</t>
+          <t>0,3</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2595,17 +2587,17 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>7,6</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2699,17 +2691,17 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>1,6</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2757,17 +2749,17 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>3,6</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2815,17 +2807,17 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>0,8</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2873,7 +2865,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -2883,7 +2875,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2931,17 +2923,17 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>0,2</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -2987,21 +2979,9 @@
       <c r="K46" t="n">
         <v>-2.483056</v>
       </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>0,0</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>1 de septiembre</t>
-        </is>
-      </c>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3047,7 +3027,7 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
@@ -3057,7 +3037,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3103,21 +3083,9 @@
       <c r="K48" t="n">
         <v>-4.754167</v>
       </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>0,0</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>1 de septiembre</t>
-        </is>
-      </c>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3163,7 +3131,7 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
@@ -3173,7 +3141,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3219,21 +3187,9 @@
       <c r="K50" t="n">
         <v>-4.010556</v>
       </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Ip</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>1 de septiembre</t>
-        </is>
-      </c>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3279,7 +3235,7 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
@@ -3289,7 +3245,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3293,7 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
@@ -3347,7 +3303,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3393,21 +3349,9 @@
       <c r="K53" t="n">
         <v>-5.735278</v>
       </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>0,0</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>1 de septiembre</t>
-        </is>
-      </c>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3453,7 +3397,7 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
@@ -3463,7 +3407,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3511,7 +3455,7 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
@@ -3521,7 +3465,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3513,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -3579,7 +3523,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3627,7 +3571,7 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
@@ -3637,7 +3581,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3629,7 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
@@ -3695,7 +3639,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3743,7 +3687,7 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
@@ -3753,7 +3697,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3801,7 +3745,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
@@ -3811,7 +3755,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3859,7 +3803,7 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
@@ -3869,7 +3813,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3917,7 +3861,7 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
@@ -3927,7 +3871,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -3975,7 +3919,7 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
@@ -3985,7 +3929,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4033,7 +3977,7 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
@@ -4043,7 +3987,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4091,13 +4035,17 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr"/>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>0,0</t>
+        </is>
+      </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4145,7 +4093,7 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
@@ -4155,7 +4103,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4203,7 +4151,7 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
@@ -4213,7 +4161,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4261,7 +4209,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -4271,7 +4219,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4319,7 +4267,7 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
@@ -4329,7 +4277,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4377,7 +4325,7 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
@@ -4387,7 +4335,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4435,7 +4383,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -4445,7 +4393,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4493,7 +4441,7 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
@@ -4503,7 +4451,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4551,7 +4499,7 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
@@ -4561,7 +4509,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4557,7 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
@@ -4619,7 +4567,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4667,7 +4615,7 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
@@ -4677,7 +4625,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4673,7 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
@@ -4735,7 +4683,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4783,17 +4731,17 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>Ip</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4841,7 +4789,7 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M78" t="inlineStr">
@@ -4851,7 +4799,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4899,7 +4847,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
@@ -4909,7 +4857,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -4957,17 +4905,17 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,2</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5015,17 +4963,17 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,1</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5073,17 +5021,17 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,7</t>
         </is>
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5131,7 +5079,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -5141,7 +5089,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5189,7 +5137,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -5199,7 +5147,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5195,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -5257,7 +5205,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5305,17 +5253,17 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,2</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5363,7 +5311,7 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M87" t="inlineStr">
@@ -5373,7 +5321,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5421,17 +5369,17 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>0,7</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5479,17 +5427,17 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>2,0</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5537,17 +5485,17 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>0,1</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5593,17 +5541,17 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>0,3</t>
+          <t>0,0</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5651,7 +5599,7 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M92" t="inlineStr">
@@ -5661,7 +5609,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5709,7 +5657,7 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
@@ -5719,7 +5667,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5767,17 +5715,17 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>Ip</t>
         </is>
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5825,7 +5773,7 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M95" t="inlineStr">
@@ -5835,7 +5783,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5883,7 +5831,7 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M96" t="inlineStr">
@@ -5893,7 +5841,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5941,17 +5889,17 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -5999,7 +5947,7 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M98" t="inlineStr">
@@ -6009,7 +5957,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>
@@ -6057,17 +6005,17 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>2025-09-01</t>
+          <t>2025-09-08</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>0,0</t>
+          <t>12,8</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>1 de septiembre</t>
+          <t>8 de septiembre</t>
         </is>
       </c>
     </row>

</xml_diff>